<commit_message>
Signed-off-by: zhufu2012 <66316168+zhufu2012@users.noreply.github.com> 【配置导出工具】 1.工具帮助文档优化 2.代码小bug修复
</commit_message>
<xml_diff>
--- a/工具帮助文档.xlsx
+++ b/工具帮助文档.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21405" windowHeight="9645"/>
+    <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="配置导出工具帮助文档" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>表格及导表工具优化需求</t>
   </si>
@@ -82,10 +82,6 @@
   </si>
   <si>
     <t>看着像报错的</t>
-  </si>
-  <si>
-    <t>计算力不足qq:2494216761
-或者你会python就自己修改</t>
   </si>
   <si>
     <t>没有反应</t>
@@ -109,7 +105,9 @@
     <t>基础配置导出工具是 用于对游戏配置进行管理的工具
 你可以使用.xlsm 或者.xls文档 来管理游戏的各类配置
 然后通过这个工具来导出成游戏中的配置。
-因为是需要导出到游戏中，所以该工具需要你的.xlsm或者.xls文件具有一定格式!!!!</t>
+因为是需要导出到游戏中，所以该工具需要你的.xlsm或者.xls文件具有一定格式!!!!
+另外，导出的配置在Configuration-Export-Tool\基础配置工具\data  这个目录哈！你可以自己再写个复制用的bat脚本
+把配置复制到游戏目录下，或者修改 复制  基础配置  到游戏目录.bat  这个bat文件里的路径</t>
   </si>
   <si>
     <t>工具全貌</t>
@@ -392,6 +390,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">具体可以看测试配置的表2 和 表3 
 基础数据类型：
 BOOL   true 或者 false    值只有两个选项时推荐使用  true 
@@ -1272,11 +1277,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1863,8 +1868,8 @@
   <sheetPr/>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:R10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2050,32 +2055,32 @@
       <c r="E15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="21" t="s">
-        <v>18</v>
+      <c r="F15" s="17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" ht="66" customHeight="1" spans="3:6">
       <c r="C16" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="17" t="s">
+    </row>
+    <row r="17" ht="55" customHeight="1" spans="3:6">
+      <c r="C17" s="21" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="17" ht="55" customHeight="1" spans="3:6">
-      <c r="C17" s="22" t="s">
-        <v>22</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" ht="22" customHeight="1"/>
@@ -2083,34 +2088,73 @@
       <c r="K19" s="34"/>
     </row>
     <row r="20" ht="17" customHeight="1"/>
-    <row r="21" ht="22" customHeight="1" spans="2:2">
-      <c r="B21" s="23" t="s">
+    <row r="21" ht="22" customHeight="1" spans="2:4">
+      <c r="B21" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" ht="43" customHeight="1" spans="2:7">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="22" ht="43" customHeight="1" spans="5:7">
-      <c r="E22" s="24" t="s">
-        <v>26</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" ht="105" customHeight="1" spans="5:5">
-      <c r="E23" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" ht="31.5" spans="5:6">
+    <row r="23" ht="105" customHeight="1" spans="2:5">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+    </row>
+    <row r="29" ht="31.5" spans="2:6">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
     </row>
-    <row r="30" ht="31.5" spans="5:6">
+    <row r="30" ht="31.5" spans="2:6">
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
     </row>
     <row r="31" ht="31.5" spans="3:6">
       <c r="C31" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="27"/>
@@ -2118,62 +2162,62 @@
     </row>
     <row r="32" ht="18.75" spans="3:4">
       <c r="C32" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="29" t="s">
         <v>29</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="34" ht="25.5" spans="3:4">
       <c r="C34" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" s="28"/>
     </row>
     <row r="35" ht="112" customHeight="1" spans="3:4">
       <c r="C35" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>32</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="46" ht="25.5" spans="3:4">
       <c r="C46" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="28"/>
     </row>
     <row r="47" ht="52" customHeight="1" spans="3:4">
       <c r="C47" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
         <v>35</v>
-      </c>
-      <c r="D47" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="48" ht="109" customHeight="1" spans="3:4">
       <c r="C48" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="49" ht="54" spans="3:4">
       <c r="C49" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="22" t="s">
         <v>39</v>
-      </c>
-      <c r="D49" s="23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="50" ht="408" customHeight="1" spans="3:4">
       <c r="C50" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="33" t="s">
         <v>41</v>
-      </c>
-      <c r="D50" s="33" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2262,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2308,7 +2352,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>

</xml_diff>